<commit_message>
added opportunity to set daily lessons amount
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/day_limits.xlsx
+++ b/src/main/resources/xlsx/day_limits.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiksanov\IdeaProjects\GA\src\main\resources\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The Diamond Doge\IdeaProjects\GA\src\main\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>11б</t>
   </si>
@@ -83,16 +83,13 @@
     <t>6в</t>
   </si>
   <si>
-    <t>Класс</t>
-  </si>
-  <si>
-    <t>Макс кол-во уроков</t>
+    <t>Класс/День недели</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,172 +436,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20">
         <v>7</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loop until success with full restart
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/day_limits.xlsx
+++ b/src/main/resources/xlsx/day_limits.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,19 +475,19 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -498,19 +498,19 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -521,19 +521,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -544,19 +544,19 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -567,19 +567,19 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -590,19 +590,19 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -613,19 +613,19 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -636,19 +636,19 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -659,19 +659,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>7</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -682,19 +682,19 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>7</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -705,19 +705,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>7</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -728,19 +728,19 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>7</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -751,19 +751,19 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>7</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -774,19 +774,19 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -797,19 +797,19 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>7</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -820,19 +820,19 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>7</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -843,19 +843,19 @@
         <v>6</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>7</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18">
         <v>5</v>
@@ -866,19 +866,19 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>7</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -889,19 +889,19 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>7</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <v>7</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20">
         <v>5</v>

</xml_diff>